<commit_message>
Add data visualization and additional experiment configurations to experiment_runner.py
</commit_message>
<xml_diff>
--- a/deney_sonuclari.xlsx
+++ b/deney_sonuclari.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -507,13 +507,13 @@
         </is>
       </c>
       <c r="G2" t="n">
-        <v>6416.598692194142</v>
+        <v>6333.67087965555</v>
       </c>
       <c r="H2" t="n">
-        <v>0</v>
+        <v>3654.90670715878</v>
       </c>
       <c r="I2" t="n">
-        <v>6397.090593233821</v>
+        <v>6383.755726392838</v>
       </c>
       <c r="J2" t="n">
         <v>280</v>
@@ -524,30 +524,30 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>100</v>
+        <v>60</v>
       </c>
       <c r="C3" t="n">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D3" t="n">
-        <v>0.9</v>
+        <v>0.8</v>
       </c>
       <c r="E3" t="n">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>(-5, -2, -8)</t>
+          <t>(-2, -3, -10)</t>
         </is>
       </c>
       <c r="G3" t="n">
-        <v>6435.461319597042</v>
+        <v>6378.306074085541</v>
       </c>
       <c r="H3" t="n">
-        <v>0</v>
+        <v>3474.424811989671</v>
       </c>
       <c r="I3" t="n">
-        <v>6378.309675289968</v>
+        <v>6323.353633624214</v>
       </c>
       <c r="J3" t="n">
         <v>280</v>
@@ -558,32 +558,66 @@
         <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>30</v>
+        <v>70</v>
       </c>
       <c r="C4" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D4" t="n">
-        <v>0.7</v>
+        <v>0.8</v>
       </c>
       <c r="E4" t="n">
-        <v>0.02</v>
+        <v>0.05</v>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>(-3, -5, -7)</t>
+          <t>(-2, -3, -10)</t>
         </is>
       </c>
       <c r="G4" t="n">
-        <v>6450.101320627629</v>
+        <v>6480.546347203733</v>
       </c>
       <c r="H4" t="n">
-        <v>0</v>
+        <v>2704.894360232138</v>
       </c>
       <c r="I4" t="n">
-        <v>6355.30763675206</v>
+        <v>6364.894360232136</v>
       </c>
       <c r="J4" t="n">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" t="n">
+        <v>80</v>
+      </c>
+      <c r="C5" t="n">
+        <v>10</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>(-2, -3, -10)</t>
+        </is>
+      </c>
+      <c r="G5" t="n">
+        <v>6356.98238963569</v>
+      </c>
+      <c r="H5" t="n">
+        <v>3226.946125835125</v>
+      </c>
+      <c r="I5" t="n">
+        <v>6353.851708818599</v>
+      </c>
+      <c r="J5" t="n">
         <v>280</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Refactor experiment parameters and add dynamic calculation for crossover and mutation rates
</commit_message>
<xml_diff>
--- a/deney_sonuclari.xlsx
+++ b/deney_sonuclari.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J5"/>
+  <dimension ref="A1:J17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -496,10 +496,10 @@
         <v>10</v>
       </c>
       <c r="D2" t="n">
-        <v>0.8</v>
+        <v>1.191</v>
       </c>
       <c r="E2" t="n">
-        <v>0.05</v>
+        <v>0.316</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
@@ -507,13 +507,13 @@
         </is>
       </c>
       <c r="G2" t="n">
-        <v>6333.67087965555</v>
+        <v>6430.903783855611</v>
       </c>
       <c r="H2" t="n">
-        <v>3654.90670715878</v>
+        <v>2661.513897768687</v>
       </c>
       <c r="I2" t="n">
-        <v>6383.755726392838</v>
+        <v>6402.32860092934</v>
       </c>
       <c r="J2" t="n">
         <v>280</v>
@@ -524,16 +524,16 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="C3" t="n">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="D3" t="n">
-        <v>0.8</v>
+        <v>1.191</v>
       </c>
       <c r="E3" t="n">
-        <v>0.05</v>
+        <v>0.141</v>
       </c>
       <c r="F3" t="inlineStr">
         <is>
@@ -541,13 +541,13 @@
         </is>
       </c>
       <c r="G3" t="n">
-        <v>6378.306074085541</v>
+        <v>6487.026814483518</v>
       </c>
       <c r="H3" t="n">
-        <v>3474.424811989671</v>
+        <v>3446.449539288811</v>
       </c>
       <c r="I3" t="n">
-        <v>6323.353633624214</v>
+        <v>6310.973671538432</v>
       </c>
       <c r="J3" t="n">
         <v>280</v>
@@ -558,16 +558,16 @@
         <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>70</v>
+        <v>50</v>
       </c>
       <c r="C4" t="n">
-        <v>10</v>
+        <v>100</v>
       </c>
       <c r="D4" t="n">
-        <v>0.8</v>
+        <v>1.191</v>
       </c>
       <c r="E4" t="n">
-        <v>0.05</v>
+        <v>0.1</v>
       </c>
       <c r="F4" t="inlineStr">
         <is>
@@ -575,13 +575,13 @@
         </is>
       </c>
       <c r="G4" t="n">
-        <v>6480.546347203733</v>
+        <v>6396.231945803867</v>
       </c>
       <c r="H4" t="n">
-        <v>2704.894360232138</v>
+        <v>3273.517367814602</v>
       </c>
       <c r="I4" t="n">
-        <v>6364.894360232136</v>
+        <v>6355.747133909991</v>
       </c>
       <c r="J4" t="n">
         <v>280</v>
@@ -592,32 +592,440 @@
         <v>4</v>
       </c>
       <c r="B5" t="n">
-        <v>80</v>
+        <v>50</v>
       </c>
       <c r="C5" t="n">
+        <v>200</v>
+      </c>
+      <c r="D5" t="n">
+        <v>1.191</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0.07099999999999999</v>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>(-2, -3, -10)</t>
+        </is>
+      </c>
+      <c r="G5" t="n">
+        <v>6461.857192319964</v>
+      </c>
+      <c r="H5" t="n">
+        <v>2545.72317992938</v>
+      </c>
+      <c r="I5" t="n">
+        <v>6318.900305878747</v>
+      </c>
+      <c r="J5" t="n">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" t="n">
+        <v>100</v>
+      </c>
+      <c r="C6" t="n">
         <v>10</v>
       </c>
-      <c r="D5" t="n">
-        <v>0.8</v>
-      </c>
-      <c r="E5" t="n">
-        <v>0.05</v>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>(-2, -3, -10)</t>
-        </is>
-      </c>
-      <c r="G5" t="n">
-        <v>6356.98238963569</v>
-      </c>
-      <c r="H5" t="n">
-        <v>3226.946125835125</v>
-      </c>
-      <c r="I5" t="n">
-        <v>6353.851708818599</v>
-      </c>
-      <c r="J5" t="n">
+      <c r="D6" t="n">
+        <v>1.261</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0.316</v>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>(-2, -3, -10)</t>
+        </is>
+      </c>
+      <c r="G6" t="n">
+        <v>6421.928887737818</v>
+      </c>
+      <c r="H6" t="n">
+        <v>2752.292209571341</v>
+      </c>
+      <c r="I6" t="n">
+        <v>6358.124382064607</v>
+      </c>
+      <c r="J6" t="n">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" t="n">
+        <v>100</v>
+      </c>
+      <c r="C7" t="n">
+        <v>50</v>
+      </c>
+      <c r="D7" t="n">
+        <v>1.261</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0.141</v>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>(-2, -3, -10)</t>
+        </is>
+      </c>
+      <c r="G7" t="n">
+        <v>6405.836051533373</v>
+      </c>
+      <c r="H7" t="n">
+        <v>3579.368005061616</v>
+      </c>
+      <c r="I7" t="n">
+        <v>6305.003425672308</v>
+      </c>
+      <c r="J7" t="n">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" t="n">
+        <v>100</v>
+      </c>
+      <c r="C8" t="n">
+        <v>100</v>
+      </c>
+      <c r="D8" t="n">
+        <v>1.261</v>
+      </c>
+      <c r="E8" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>(-2, -3, -10)</t>
+        </is>
+      </c>
+      <c r="G8" t="n">
+        <v>6438.481335196971</v>
+      </c>
+      <c r="H8" t="n">
+        <v>3001.695682825894</v>
+      </c>
+      <c r="I8" t="n">
+        <v>6270.45400907426</v>
+      </c>
+      <c r="J8" t="n">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" t="n">
+        <v>100</v>
+      </c>
+      <c r="C9" t="n">
+        <v>200</v>
+      </c>
+      <c r="D9" t="n">
+        <v>1.261</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0.07099999999999999</v>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>(-2, -3, -10)</t>
+        </is>
+      </c>
+      <c r="G9" t="n">
+        <v>6427.693220095725</v>
+      </c>
+      <c r="H9" t="n">
+        <v>2578.315197740972</v>
+      </c>
+      <c r="I9" t="n">
+        <v>6300.708048426569</v>
+      </c>
+      <c r="J9" t="n">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" t="n">
+        <v>150</v>
+      </c>
+      <c r="C10" t="n">
+        <v>10</v>
+      </c>
+      <c r="D10" t="n">
+        <v>1.301</v>
+      </c>
+      <c r="E10" t="n">
+        <v>0.316</v>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>(-2, -3, -10)</t>
+        </is>
+      </c>
+      <c r="G10" t="n">
+        <v>6460.461252407366</v>
+      </c>
+      <c r="H10" t="n">
+        <v>2974.980946830065</v>
+      </c>
+      <c r="I10" t="n">
+        <v>6410.652579342721</v>
+      </c>
+      <c r="J10" t="n">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" t="n">
+        <v>150</v>
+      </c>
+      <c r="C11" t="n">
+        <v>50</v>
+      </c>
+      <c r="D11" t="n">
+        <v>1.301</v>
+      </c>
+      <c r="E11" t="n">
+        <v>0.141</v>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>(-2, -3, -10)</t>
+        </is>
+      </c>
+      <c r="G11" t="n">
+        <v>6357.430453075702</v>
+      </c>
+      <c r="H11" t="n">
+        <v>2962.33533298378</v>
+      </c>
+      <c r="I11" t="n">
+        <v>6321.80880149837</v>
+      </c>
+      <c r="J11" t="n">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" t="n">
+        <v>150</v>
+      </c>
+      <c r="C12" t="n">
+        <v>100</v>
+      </c>
+      <c r="D12" t="n">
+        <v>1.301</v>
+      </c>
+      <c r="E12" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>(-2, -3, -10)</t>
+        </is>
+      </c>
+      <c r="G12" t="n">
+        <v>6407.39492048641</v>
+      </c>
+      <c r="H12" t="n">
+        <v>2810.527906002668</v>
+      </c>
+      <c r="I12" t="n">
+        <v>6297.908681315195</v>
+      </c>
+      <c r="J12" t="n">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" t="n">
+        <v>150</v>
+      </c>
+      <c r="C13" t="n">
+        <v>200</v>
+      </c>
+      <c r="D13" t="n">
+        <v>1.301</v>
+      </c>
+      <c r="E13" t="n">
+        <v>0.07099999999999999</v>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>(-2, -3, -10)</t>
+        </is>
+      </c>
+      <c r="G13" t="n">
+        <v>6376.158185460904</v>
+      </c>
+      <c r="H13" t="n">
+        <v>2926.56359130191</v>
+      </c>
+      <c r="I13" t="n">
+        <v>6244.618389071275</v>
+      </c>
+      <c r="J13" t="n">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>13</v>
+      </c>
+      <c r="B14" t="n">
+        <v>200</v>
+      </c>
+      <c r="C14" t="n">
+        <v>10</v>
+      </c>
+      <c r="D14" t="n">
+        <v>1.33</v>
+      </c>
+      <c r="E14" t="n">
+        <v>0.316</v>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>(-2, -3, -10)</t>
+        </is>
+      </c>
+      <c r="G14" t="n">
+        <v>6425.265875087587</v>
+      </c>
+      <c r="H14" t="n">
+        <v>3008.761377258846</v>
+      </c>
+      <c r="I14" t="n">
+        <v>6327.74590398671</v>
+      </c>
+      <c r="J14" t="n">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>14</v>
+      </c>
+      <c r="B15" t="n">
+        <v>200</v>
+      </c>
+      <c r="C15" t="n">
+        <v>50</v>
+      </c>
+      <c r="D15" t="n">
+        <v>1.33</v>
+      </c>
+      <c r="E15" t="n">
+        <v>0.141</v>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>(-2, -3, -10)</t>
+        </is>
+      </c>
+      <c r="G15" t="n">
+        <v>6370.464144974343</v>
+      </c>
+      <c r="H15" t="n">
+        <v>3299.360630169088</v>
+      </c>
+      <c r="I15" t="n">
+        <v>6329.273835921167</v>
+      </c>
+      <c r="J15" t="n">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>15</v>
+      </c>
+      <c r="B16" t="n">
+        <v>200</v>
+      </c>
+      <c r="C16" t="n">
+        <v>100</v>
+      </c>
+      <c r="D16" t="n">
+        <v>1.33</v>
+      </c>
+      <c r="E16" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>(-2, -3, -10)</t>
+        </is>
+      </c>
+      <c r="G16" t="n">
+        <v>6392.628228112985</v>
+      </c>
+      <c r="H16" t="n">
+        <v>2768.444900400293</v>
+      </c>
+      <c r="I16" t="n">
+        <v>6303.592792956696</v>
+      </c>
+      <c r="J16" t="n">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>16</v>
+      </c>
+      <c r="B17" t="n">
+        <v>200</v>
+      </c>
+      <c r="C17" t="n">
+        <v>200</v>
+      </c>
+      <c r="D17" t="n">
+        <v>1.33</v>
+      </c>
+      <c r="E17" t="n">
+        <v>0.07099999999999999</v>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>(-2, -3, -10)</t>
+        </is>
+      </c>
+      <c r="G17" t="n">
+        <v>6453.684345521685</v>
+      </c>
+      <c r="H17" t="n">
+        <v>2848.611804193922</v>
+      </c>
+      <c r="I17" t="n">
+        <v>6319.97599708213</v>
+      </c>
+      <c r="J17" t="n">
         <v>280</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update experiment parameters and enhance data normalization and visualization
</commit_message>
<xml_diff>
--- a/deney_sonuclari.xlsx
+++ b/deney_sonuclari.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J17"/>
+  <dimension ref="A1:J64"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -490,16 +490,16 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>50</v>
+        <v>5</v>
       </c>
       <c r="C2" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="D2" t="n">
-        <v>1.191</v>
+        <v>0.961</v>
       </c>
       <c r="E2" t="n">
-        <v>0.316</v>
+        <v>1</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
@@ -507,13 +507,13 @@
         </is>
       </c>
       <c r="G2" t="n">
-        <v>6430.903783855611</v>
+        <v>6518.861507568927</v>
       </c>
       <c r="H2" t="n">
-        <v>2661.513897768687</v>
+        <v>2581.925303500336</v>
       </c>
       <c r="I2" t="n">
-        <v>6402.32860092934</v>
+        <v>6560.494307640918</v>
       </c>
       <c r="J2" t="n">
         <v>280</v>
@@ -524,16 +524,16 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>50</v>
+        <v>5</v>
       </c>
       <c r="C3" t="n">
-        <v>50</v>
+        <v>5</v>
       </c>
       <c r="D3" t="n">
-        <v>1.191</v>
+        <v>0.961</v>
       </c>
       <c r="E3" t="n">
-        <v>0.141</v>
+        <v>0.447</v>
       </c>
       <c r="F3" t="inlineStr">
         <is>
@@ -541,13 +541,13 @@
         </is>
       </c>
       <c r="G3" t="n">
-        <v>6487.026814483518</v>
+        <v>6685.352207531851</v>
       </c>
       <c r="H3" t="n">
-        <v>3446.449539288811</v>
+        <v>2973.852876597616</v>
       </c>
       <c r="I3" t="n">
-        <v>6310.973671538432</v>
+        <v>6468.83958063655</v>
       </c>
       <c r="J3" t="n">
         <v>280</v>
@@ -558,16 +558,16 @@
         <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>50</v>
+        <v>5</v>
       </c>
       <c r="C4" t="n">
-        <v>100</v>
+        <v>10</v>
       </c>
       <c r="D4" t="n">
-        <v>1.191</v>
+        <v>0.961</v>
       </c>
       <c r="E4" t="n">
-        <v>0.1</v>
+        <v>0.316</v>
       </c>
       <c r="F4" t="inlineStr">
         <is>
@@ -575,13 +575,13 @@
         </is>
       </c>
       <c r="G4" t="n">
-        <v>6396.231945803867</v>
+        <v>6714.511708590644</v>
       </c>
       <c r="H4" t="n">
-        <v>3273.517367814602</v>
+        <v>3351.240423652248</v>
       </c>
       <c r="I4" t="n">
-        <v>6355.747133909991</v>
+        <v>6461.732078267617</v>
       </c>
       <c r="J4" t="n">
         <v>280</v>
@@ -592,16 +592,16 @@
         <v>4</v>
       </c>
       <c r="B5" t="n">
-        <v>50</v>
+        <v>5</v>
       </c>
       <c r="C5" t="n">
-        <v>200</v>
+        <v>20</v>
       </c>
       <c r="D5" t="n">
-        <v>1.191</v>
+        <v>0.961</v>
       </c>
       <c r="E5" t="n">
-        <v>0.07099999999999999</v>
+        <v>0.224</v>
       </c>
       <c r="F5" t="inlineStr">
         <is>
@@ -609,13 +609,13 @@
         </is>
       </c>
       <c r="G5" t="n">
-        <v>6461.857192319964</v>
+        <v>6500.247505130281</v>
       </c>
       <c r="H5" t="n">
-        <v>2545.72317992938</v>
+        <v>2408.6068987115</v>
       </c>
       <c r="I5" t="n">
-        <v>6318.900305878747</v>
+        <v>6485.647373970398</v>
       </c>
       <c r="J5" t="n">
         <v>280</v>
@@ -626,16 +626,16 @@
         <v>5</v>
       </c>
       <c r="B6" t="n">
-        <v>100</v>
+        <v>5</v>
       </c>
       <c r="C6" t="n">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="D6" t="n">
-        <v>1.261</v>
+        <v>0.961</v>
       </c>
       <c r="E6" t="n">
-        <v>0.316</v>
+        <v>0.141</v>
       </c>
       <c r="F6" t="inlineStr">
         <is>
@@ -643,13 +643,13 @@
         </is>
       </c>
       <c r="G6" t="n">
-        <v>6421.928887737818</v>
+        <v>6608.843420239962</v>
       </c>
       <c r="H6" t="n">
-        <v>2752.292209571341</v>
+        <v>2779.795878774753</v>
       </c>
       <c r="I6" t="n">
-        <v>6358.124382064607</v>
+        <v>6381.339101396176</v>
       </c>
       <c r="J6" t="n">
         <v>280</v>
@@ -660,16 +660,16 @@
         <v>6</v>
       </c>
       <c r="B7" t="n">
+        <v>5</v>
+      </c>
+      <c r="C7" t="n">
         <v>100</v>
       </c>
-      <c r="C7" t="n">
-        <v>50</v>
-      </c>
       <c r="D7" t="n">
-        <v>1.261</v>
+        <v>0.961</v>
       </c>
       <c r="E7" t="n">
-        <v>0.141</v>
+        <v>0.1</v>
       </c>
       <c r="F7" t="inlineStr">
         <is>
@@ -677,13 +677,13 @@
         </is>
       </c>
       <c r="G7" t="n">
-        <v>6405.836051533373</v>
+        <v>6374.626453014844</v>
       </c>
       <c r="H7" t="n">
-        <v>3579.368005061616</v>
+        <v>2948.952156234473</v>
       </c>
       <c r="I7" t="n">
-        <v>6305.003425672308</v>
+        <v>6382.948214895344</v>
       </c>
       <c r="J7" t="n">
         <v>280</v>
@@ -694,16 +694,16 @@
         <v>7</v>
       </c>
       <c r="B8" t="n">
-        <v>100</v>
+        <v>5</v>
       </c>
       <c r="C8" t="n">
-        <v>100</v>
+        <v>250</v>
       </c>
       <c r="D8" t="n">
-        <v>1.261</v>
+        <v>0.961</v>
       </c>
       <c r="E8" t="n">
-        <v>0.1</v>
+        <v>0.063</v>
       </c>
       <c r="F8" t="inlineStr">
         <is>
@@ -711,13 +711,13 @@
         </is>
       </c>
       <c r="G8" t="n">
-        <v>6438.481335196971</v>
+        <v>6541.998336051903</v>
       </c>
       <c r="H8" t="n">
-        <v>3001.695682825894</v>
+        <v>3958.871192964758</v>
       </c>
       <c r="I8" t="n">
-        <v>6270.45400907426</v>
+        <v>6321.3722183634</v>
       </c>
       <c r="J8" t="n">
         <v>280</v>
@@ -728,16 +728,16 @@
         <v>8</v>
       </c>
       <c r="B9" t="n">
-        <v>100</v>
+        <v>10</v>
       </c>
       <c r="C9" t="n">
-        <v>200</v>
+        <v>1</v>
       </c>
       <c r="D9" t="n">
-        <v>1.261</v>
+        <v>1.03</v>
       </c>
       <c r="E9" t="n">
-        <v>0.07099999999999999</v>
+        <v>1</v>
       </c>
       <c r="F9" t="inlineStr">
         <is>
@@ -745,13 +745,13 @@
         </is>
       </c>
       <c r="G9" t="n">
-        <v>6427.693220095725</v>
+        <v>6506.62083311509</v>
       </c>
       <c r="H9" t="n">
-        <v>2578.315197740972</v>
+        <v>2524.78912872877</v>
       </c>
       <c r="I9" t="n">
-        <v>6300.708048426569</v>
+        <v>6525.831243219104</v>
       </c>
       <c r="J9" t="n">
         <v>280</v>
@@ -762,16 +762,16 @@
         <v>9</v>
       </c>
       <c r="B10" t="n">
-        <v>150</v>
+        <v>10</v>
       </c>
       <c r="C10" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D10" t="n">
-        <v>1.301</v>
+        <v>1.03</v>
       </c>
       <c r="E10" t="n">
-        <v>0.316</v>
+        <v>0.447</v>
       </c>
       <c r="F10" t="inlineStr">
         <is>
@@ -779,13 +779,13 @@
         </is>
       </c>
       <c r="G10" t="n">
-        <v>6460.461252407366</v>
+        <v>6588.465786945528</v>
       </c>
       <c r="H10" t="n">
-        <v>2974.980946830065</v>
+        <v>2676.134926856482</v>
       </c>
       <c r="I10" t="n">
-        <v>6410.652579342721</v>
+        <v>6449.207856036227</v>
       </c>
       <c r="J10" t="n">
         <v>280</v>
@@ -796,16 +796,16 @@
         <v>10</v>
       </c>
       <c r="B11" t="n">
-        <v>150</v>
+        <v>10</v>
       </c>
       <c r="C11" t="n">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="D11" t="n">
-        <v>1.301</v>
+        <v>1.03</v>
       </c>
       <c r="E11" t="n">
-        <v>0.141</v>
+        <v>0.316</v>
       </c>
       <c r="F11" t="inlineStr">
         <is>
@@ -813,13 +813,13 @@
         </is>
       </c>
       <c r="G11" t="n">
-        <v>6357.430453075702</v>
+        <v>6484.418370796331</v>
       </c>
       <c r="H11" t="n">
-        <v>2962.33533298378</v>
+        <v>2877.009220325039</v>
       </c>
       <c r="I11" t="n">
-        <v>6321.80880149837</v>
+        <v>6425.385963645234</v>
       </c>
       <c r="J11" t="n">
         <v>280</v>
@@ -830,16 +830,16 @@
         <v>11</v>
       </c>
       <c r="B12" t="n">
-        <v>150</v>
+        <v>10</v>
       </c>
       <c r="C12" t="n">
-        <v>100</v>
+        <v>20</v>
       </c>
       <c r="D12" t="n">
-        <v>1.301</v>
+        <v>1.03</v>
       </c>
       <c r="E12" t="n">
-        <v>0.1</v>
+        <v>0.224</v>
       </c>
       <c r="F12" t="inlineStr">
         <is>
@@ -847,13 +847,13 @@
         </is>
       </c>
       <c r="G12" t="n">
-        <v>6407.39492048641</v>
+        <v>6368.678500280729</v>
       </c>
       <c r="H12" t="n">
-        <v>2810.527906002668</v>
+        <v>3247.62000364887</v>
       </c>
       <c r="I12" t="n">
-        <v>6297.908681315195</v>
+        <v>6423.441837853322</v>
       </c>
       <c r="J12" t="n">
         <v>280</v>
@@ -864,16 +864,16 @@
         <v>12</v>
       </c>
       <c r="B13" t="n">
-        <v>150</v>
+        <v>10</v>
       </c>
       <c r="C13" t="n">
-        <v>200</v>
+        <v>50</v>
       </c>
       <c r="D13" t="n">
-        <v>1.301</v>
+        <v>1.03</v>
       </c>
       <c r="E13" t="n">
-        <v>0.07099999999999999</v>
+        <v>0.141</v>
       </c>
       <c r="F13" t="inlineStr">
         <is>
@@ -881,13 +881,13 @@
         </is>
       </c>
       <c r="G13" t="n">
-        <v>6376.158185460904</v>
+        <v>6450.89769865422</v>
       </c>
       <c r="H13" t="n">
-        <v>2926.56359130191</v>
+        <v>3186.948214084469</v>
       </c>
       <c r="I13" t="n">
-        <v>6244.618389071275</v>
+        <v>6346.129957579063</v>
       </c>
       <c r="J13" t="n">
         <v>280</v>
@@ -898,16 +898,16 @@
         <v>13</v>
       </c>
       <c r="B14" t="n">
-        <v>200</v>
+        <v>10</v>
       </c>
       <c r="C14" t="n">
-        <v>10</v>
+        <v>100</v>
       </c>
       <c r="D14" t="n">
-        <v>1.33</v>
+        <v>1.03</v>
       </c>
       <c r="E14" t="n">
-        <v>0.316</v>
+        <v>0.1</v>
       </c>
       <c r="F14" t="inlineStr">
         <is>
@@ -915,13 +915,13 @@
         </is>
       </c>
       <c r="G14" t="n">
-        <v>6425.265875087587</v>
+        <v>6447.384761490687</v>
       </c>
       <c r="H14" t="n">
-        <v>3008.761377258846</v>
+        <v>3281.587685560629</v>
       </c>
       <c r="I14" t="n">
-        <v>6327.74590398671</v>
+        <v>6376.376108154289</v>
       </c>
       <c r="J14" t="n">
         <v>280</v>
@@ -932,16 +932,16 @@
         <v>14</v>
       </c>
       <c r="B15" t="n">
-        <v>200</v>
+        <v>10</v>
       </c>
       <c r="C15" t="n">
-        <v>50</v>
+        <v>250</v>
       </c>
       <c r="D15" t="n">
-        <v>1.33</v>
+        <v>1.03</v>
       </c>
       <c r="E15" t="n">
-        <v>0.141</v>
+        <v>0.063</v>
       </c>
       <c r="F15" t="inlineStr">
         <is>
@@ -949,13 +949,13 @@
         </is>
       </c>
       <c r="G15" t="n">
-        <v>6370.464144974343</v>
+        <v>6539.994993724745</v>
       </c>
       <c r="H15" t="n">
-        <v>3299.360630169088</v>
+        <v>3105.597668839656</v>
       </c>
       <c r="I15" t="n">
-        <v>6329.273835921167</v>
+        <v>6320.015491924987</v>
       </c>
       <c r="J15" t="n">
         <v>280</v>
@@ -966,16 +966,16 @@
         <v>15</v>
       </c>
       <c r="B16" t="n">
-        <v>200</v>
+        <v>15</v>
       </c>
       <c r="C16" t="n">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="D16" t="n">
-        <v>1.33</v>
+        <v>1.071</v>
       </c>
       <c r="E16" t="n">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="F16" t="inlineStr">
         <is>
@@ -983,13 +983,13 @@
         </is>
       </c>
       <c r="G16" t="n">
-        <v>6392.628228112985</v>
+        <v>6505.122907472884</v>
       </c>
       <c r="H16" t="n">
-        <v>2768.444900400293</v>
+        <v>2948.569223689222</v>
       </c>
       <c r="I16" t="n">
-        <v>6303.592792956696</v>
+        <v>6459.35502044272</v>
       </c>
       <c r="J16" t="n">
         <v>280</v>
@@ -1000,16 +1000,16 @@
         <v>16</v>
       </c>
       <c r="B17" t="n">
-        <v>200</v>
+        <v>15</v>
       </c>
       <c r="C17" t="n">
-        <v>200</v>
+        <v>5</v>
       </c>
       <c r="D17" t="n">
-        <v>1.33</v>
+        <v>1.071</v>
       </c>
       <c r="E17" t="n">
-        <v>0.07099999999999999</v>
+        <v>0.447</v>
       </c>
       <c r="F17" t="inlineStr">
         <is>
@@ -1017,15 +1017,1613 @@
         </is>
       </c>
       <c r="G17" t="n">
-        <v>6453.684345521685</v>
+        <v>6472.014799967113</v>
       </c>
       <c r="H17" t="n">
-        <v>2848.611804193922</v>
+        <v>3172.576070462766</v>
       </c>
       <c r="I17" t="n">
-        <v>6319.97599708213</v>
+        <v>6480.429393806795</v>
       </c>
       <c r="J17" t="n">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>17</v>
+      </c>
+      <c r="B18" t="n">
+        <v>15</v>
+      </c>
+      <c r="C18" t="n">
+        <v>10</v>
+      </c>
+      <c r="D18" t="n">
+        <v>1.071</v>
+      </c>
+      <c r="E18" t="n">
+        <v>0.316</v>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>(-2, -3, -10)</t>
+        </is>
+      </c>
+      <c r="G18" t="n">
+        <v>6465.522715878295</v>
+      </c>
+      <c r="H18" t="n">
+        <v>2992.16872174256</v>
+      </c>
+      <c r="I18" t="n">
+        <v>6441.365620019395</v>
+      </c>
+      <c r="J18" t="n">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>18</v>
+      </c>
+      <c r="B19" t="n">
+        <v>15</v>
+      </c>
+      <c r="C19" t="n">
+        <v>20</v>
+      </c>
+      <c r="D19" t="n">
+        <v>1.071</v>
+      </c>
+      <c r="E19" t="n">
+        <v>0.224</v>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>(-2, -3, -10)</t>
+        </is>
+      </c>
+      <c r="G19" t="n">
+        <v>6564.376434881039</v>
+      </c>
+      <c r="H19" t="n">
+        <v>2775.247048932445</v>
+      </c>
+      <c r="I19" t="n">
+        <v>6423.227850045214</v>
+      </c>
+      <c r="J19" t="n">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>19</v>
+      </c>
+      <c r="B20" t="n">
+        <v>15</v>
+      </c>
+      <c r="C20" t="n">
+        <v>50</v>
+      </c>
+      <c r="D20" t="n">
+        <v>1.071</v>
+      </c>
+      <c r="E20" t="n">
+        <v>0.141</v>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>(-2, -3, -10)</t>
+        </is>
+      </c>
+      <c r="G20" t="n">
+        <v>6531.032825109653</v>
+      </c>
+      <c r="H20" t="n">
+        <v>2729.709776118199</v>
+      </c>
+      <c r="I20" t="n">
+        <v>6392.100024133892</v>
+      </c>
+      <c r="J20" t="n">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>20</v>
+      </c>
+      <c r="B21" t="n">
+        <v>15</v>
+      </c>
+      <c r="C21" t="n">
+        <v>100</v>
+      </c>
+      <c r="D21" t="n">
+        <v>1.071</v>
+      </c>
+      <c r="E21" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>(-2, -3, -10)</t>
+        </is>
+      </c>
+      <c r="G21" t="n">
+        <v>6534.355535027148</v>
+      </c>
+      <c r="H21" t="n">
+        <v>2592.800200857949</v>
+      </c>
+      <c r="I21" t="n">
+        <v>6398.558936886784</v>
+      </c>
+      <c r="J21" t="n">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>21</v>
+      </c>
+      <c r="B22" t="n">
+        <v>15</v>
+      </c>
+      <c r="C22" t="n">
+        <v>250</v>
+      </c>
+      <c r="D22" t="n">
+        <v>1.071</v>
+      </c>
+      <c r="E22" t="n">
+        <v>0.063</v>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>(-2, -3, -10)</t>
+        </is>
+      </c>
+      <c r="G22" t="n">
+        <v>6353.487072274862</v>
+      </c>
+      <c r="H22" t="n">
+        <v>3419.098241656744</v>
+      </c>
+      <c r="I22" t="n">
+        <v>6332.203511346804</v>
+      </c>
+      <c r="J22" t="n">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>22</v>
+      </c>
+      <c r="B23" t="n">
+        <v>20</v>
+      </c>
+      <c r="C23" t="n">
+        <v>1</v>
+      </c>
+      <c r="D23" t="n">
+        <v>1.1</v>
+      </c>
+      <c r="E23" t="n">
+        <v>1</v>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>(-2, -3, -10)</t>
+        </is>
+      </c>
+      <c r="G23" t="n">
+        <v>6525.479339426021</v>
+      </c>
+      <c r="H23" t="n">
+        <v>2323.096204002819</v>
+      </c>
+      <c r="I23" t="n">
+        <v>6486.086128343104</v>
+      </c>
+      <c r="J23" t="n">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>23</v>
+      </c>
+      <c r="B24" t="n">
+        <v>20</v>
+      </c>
+      <c r="C24" t="n">
+        <v>5</v>
+      </c>
+      <c r="D24" t="n">
+        <v>1.1</v>
+      </c>
+      <c r="E24" t="n">
+        <v>0.447</v>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>(-2, -3, -10)</t>
+        </is>
+      </c>
+      <c r="G24" t="n">
+        <v>6378.287367123337</v>
+      </c>
+      <c r="H24" t="n">
+        <v>2471.868449191394</v>
+      </c>
+      <c r="I24" t="n">
+        <v>6424.070876920905</v>
+      </c>
+      <c r="J24" t="n">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>24</v>
+      </c>
+      <c r="B25" t="n">
+        <v>20</v>
+      </c>
+      <c r="C25" t="n">
+        <v>10</v>
+      </c>
+      <c r="D25" t="n">
+        <v>1.1</v>
+      </c>
+      <c r="E25" t="n">
+        <v>0.316</v>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>(-2, -3, -10)</t>
+        </is>
+      </c>
+      <c r="G25" t="n">
+        <v>6418.81863714576</v>
+      </c>
+      <c r="H25" t="n">
+        <v>2692.426428836886</v>
+      </c>
+      <c r="I25" t="n">
+        <v>6399.511610246236</v>
+      </c>
+      <c r="J25" t="n">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>25</v>
+      </c>
+      <c r="B26" t="n">
+        <v>20</v>
+      </c>
+      <c r="C26" t="n">
+        <v>20</v>
+      </c>
+      <c r="D26" t="n">
+        <v>1.1</v>
+      </c>
+      <c r="E26" t="n">
+        <v>0.224</v>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>(-2, -3, -10)</t>
+        </is>
+      </c>
+      <c r="G26" t="n">
+        <v>6571.433924648599</v>
+      </c>
+      <c r="H26" t="n">
+        <v>2624.551752761246</v>
+      </c>
+      <c r="I26" t="n">
+        <v>6418.77689986613</v>
+      </c>
+      <c r="J26" t="n">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>26</v>
+      </c>
+      <c r="B27" t="n">
+        <v>20</v>
+      </c>
+      <c r="C27" t="n">
+        <v>50</v>
+      </c>
+      <c r="D27" t="n">
+        <v>1.1</v>
+      </c>
+      <c r="E27" t="n">
+        <v>0.141</v>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>(-2, -3, -10)</t>
+        </is>
+      </c>
+      <c r="G27" t="n">
+        <v>6528.909219428319</v>
+      </c>
+      <c r="H27" t="n">
+        <v>2671.222989309911</v>
+      </c>
+      <c r="I27" t="n">
+        <v>6346.632341899576</v>
+      </c>
+      <c r="J27" t="n">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>27</v>
+      </c>
+      <c r="B28" t="n">
+        <v>20</v>
+      </c>
+      <c r="C28" t="n">
+        <v>100</v>
+      </c>
+      <c r="D28" t="n">
+        <v>1.1</v>
+      </c>
+      <c r="E28" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>(-2, -3, -10)</t>
+        </is>
+      </c>
+      <c r="G28" t="n">
+        <v>6450.985580989009</v>
+      </c>
+      <c r="H28" t="n">
+        <v>3134.051261385959</v>
+      </c>
+      <c r="I28" t="n">
+        <v>6314.864798796764</v>
+      </c>
+      <c r="J28" t="n">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>28</v>
+      </c>
+      <c r="B29" t="n">
+        <v>20</v>
+      </c>
+      <c r="C29" t="n">
+        <v>250</v>
+      </c>
+      <c r="D29" t="n">
+        <v>1.1</v>
+      </c>
+      <c r="E29" t="n">
+        <v>0.063</v>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>(-2, -3, -10)</t>
+        </is>
+      </c>
+      <c r="G29" t="n">
+        <v>6430.333537080361</v>
+      </c>
+      <c r="H29" t="n">
+        <v>3462.69123261639</v>
+      </c>
+      <c r="I29" t="n">
+        <v>6341.224924647181</v>
+      </c>
+      <c r="J29" t="n">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>29</v>
+      </c>
+      <c r="B30" t="n">
+        <v>25</v>
+      </c>
+      <c r="C30" t="n">
+        <v>1</v>
+      </c>
+      <c r="D30" t="n">
+        <v>1.122</v>
+      </c>
+      <c r="E30" t="n">
+        <v>1</v>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>(-2, -3, -10)</t>
+        </is>
+      </c>
+      <c r="G30" t="n">
+        <v>6398.46377801039</v>
+      </c>
+      <c r="H30" t="n">
+        <v>2939.938050146161</v>
+      </c>
+      <c r="I30" t="n">
+        <v>6472.171255912724</v>
+      </c>
+      <c r="J30" t="n">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>30</v>
+      </c>
+      <c r="B31" t="n">
+        <v>25</v>
+      </c>
+      <c r="C31" t="n">
+        <v>5</v>
+      </c>
+      <c r="D31" t="n">
+        <v>1.122</v>
+      </c>
+      <c r="E31" t="n">
+        <v>0.447</v>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>(-2, -3, -10)</t>
+        </is>
+      </c>
+      <c r="G31" t="n">
+        <v>6478.559216898567</v>
+      </c>
+      <c r="H31" t="n">
+        <v>2837.70378691324</v>
+      </c>
+      <c r="I31" t="n">
+        <v>6402.681476436537</v>
+      </c>
+      <c r="J31" t="n">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>31</v>
+      </c>
+      <c r="B32" t="n">
+        <v>25</v>
+      </c>
+      <c r="C32" t="n">
+        <v>10</v>
+      </c>
+      <c r="D32" t="n">
+        <v>1.122</v>
+      </c>
+      <c r="E32" t="n">
+        <v>0.316</v>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>(-2, -3, -10)</t>
+        </is>
+      </c>
+      <c r="G32" t="n">
+        <v>6472.416244916344</v>
+      </c>
+      <c r="H32" t="n">
+        <v>3066.331151964251</v>
+      </c>
+      <c r="I32" t="n">
+        <v>6360.288972259594</v>
+      </c>
+      <c r="J32" t="n">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>32</v>
+      </c>
+      <c r="B33" t="n">
+        <v>25</v>
+      </c>
+      <c r="C33" t="n">
+        <v>20</v>
+      </c>
+      <c r="D33" t="n">
+        <v>1.122</v>
+      </c>
+      <c r="E33" t="n">
+        <v>0.224</v>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>(-2, -3, -10)</t>
+        </is>
+      </c>
+      <c r="G33" t="n">
+        <v>6477.894336310983</v>
+      </c>
+      <c r="H33" t="n">
+        <v>3418.884854865454</v>
+      </c>
+      <c r="I33" t="n">
+        <v>6361.008782855609</v>
+      </c>
+      <c r="J33" t="n">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>33</v>
+      </c>
+      <c r="B34" t="n">
+        <v>25</v>
+      </c>
+      <c r="C34" t="n">
+        <v>50</v>
+      </c>
+      <c r="D34" t="n">
+        <v>1.122</v>
+      </c>
+      <c r="E34" t="n">
+        <v>0.141</v>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>(-2, -3, -10)</t>
+        </is>
+      </c>
+      <c r="G34" t="n">
+        <v>6484.532390056156</v>
+      </c>
+      <c r="H34" t="n">
+        <v>2922.92754989156</v>
+      </c>
+      <c r="I34" t="n">
+        <v>6340.622724943464</v>
+      </c>
+      <c r="J34" t="n">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>34</v>
+      </c>
+      <c r="B35" t="n">
+        <v>25</v>
+      </c>
+      <c r="C35" t="n">
+        <v>100</v>
+      </c>
+      <c r="D35" t="n">
+        <v>1.122</v>
+      </c>
+      <c r="E35" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>(-2, -3, -10)</t>
+        </is>
+      </c>
+      <c r="G35" t="n">
+        <v>6438.195973401374</v>
+      </c>
+      <c r="H35" t="n">
+        <v>2762.567375852587</v>
+      </c>
+      <c r="I35" t="n">
+        <v>6298.784476087911</v>
+      </c>
+      <c r="J35" t="n">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>35</v>
+      </c>
+      <c r="B36" t="n">
+        <v>25</v>
+      </c>
+      <c r="C36" t="n">
+        <v>250</v>
+      </c>
+      <c r="D36" t="n">
+        <v>1.122</v>
+      </c>
+      <c r="E36" t="n">
+        <v>0.063</v>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>(-2, -3, -10)</t>
+        </is>
+      </c>
+      <c r="G36" t="n">
+        <v>6495.925155155358</v>
+      </c>
+      <c r="H36" t="n">
+        <v>2721.977395572215</v>
+      </c>
+      <c r="I36" t="n">
+        <v>6259.085005046529</v>
+      </c>
+      <c r="J36" t="n">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>36</v>
+      </c>
+      <c r="B37" t="n">
+        <v>30</v>
+      </c>
+      <c r="C37" t="n">
+        <v>1</v>
+      </c>
+      <c r="D37" t="n">
+        <v>1.14</v>
+      </c>
+      <c r="E37" t="n">
+        <v>1</v>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>(-2, -3, -10)</t>
+        </is>
+      </c>
+      <c r="G37" t="n">
+        <v>6495.370567080535</v>
+      </c>
+      <c r="H37" t="n">
+        <v>3646.654914157904</v>
+      </c>
+      <c r="I37" t="n">
+        <v>6437.51958338615</v>
+      </c>
+      <c r="J37" t="n">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>37</v>
+      </c>
+      <c r="B38" t="n">
+        <v>30</v>
+      </c>
+      <c r="C38" t="n">
+        <v>5</v>
+      </c>
+      <c r="D38" t="n">
+        <v>1.14</v>
+      </c>
+      <c r="E38" t="n">
+        <v>0.447</v>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>(-2, -3, -10)</t>
+        </is>
+      </c>
+      <c r="G38" t="n">
+        <v>6527.04048073993</v>
+      </c>
+      <c r="H38" t="n">
+        <v>2881.504992983299</v>
+      </c>
+      <c r="I38" t="n">
+        <v>6489.78611999584</v>
+      </c>
+      <c r="J38" t="n">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>38</v>
+      </c>
+      <c r="B39" t="n">
+        <v>30</v>
+      </c>
+      <c r="C39" t="n">
+        <v>10</v>
+      </c>
+      <c r="D39" t="n">
+        <v>1.14</v>
+      </c>
+      <c r="E39" t="n">
+        <v>0.316</v>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>(-2, -3, -10)</t>
+        </is>
+      </c>
+      <c r="G39" t="n">
+        <v>6394.37653475156</v>
+      </c>
+      <c r="H39" t="n">
+        <v>3703.927494232278</v>
+      </c>
+      <c r="I39" t="n">
+        <v>6360.083495116339</v>
+      </c>
+      <c r="J39" t="n">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>39</v>
+      </c>
+      <c r="B40" t="n">
+        <v>30</v>
+      </c>
+      <c r="C40" t="n">
+        <v>20</v>
+      </c>
+      <c r="D40" t="n">
+        <v>1.14</v>
+      </c>
+      <c r="E40" t="n">
+        <v>0.224</v>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>(-2, -3, -10)</t>
+        </is>
+      </c>
+      <c r="G40" t="n">
+        <v>6430.077325089475</v>
+      </c>
+      <c r="H40" t="n">
+        <v>2872.654330247189</v>
+      </c>
+      <c r="I40" t="n">
+        <v>6311.548446326268</v>
+      </c>
+      <c r="J40" t="n">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>40</v>
+      </c>
+      <c r="B41" t="n">
+        <v>30</v>
+      </c>
+      <c r="C41" t="n">
+        <v>50</v>
+      </c>
+      <c r="D41" t="n">
+        <v>1.14</v>
+      </c>
+      <c r="E41" t="n">
+        <v>0.141</v>
+      </c>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>(-2, -3, -10)</t>
+        </is>
+      </c>
+      <c r="G41" t="n">
+        <v>6426.478040960575</v>
+      </c>
+      <c r="H41" t="n">
+        <v>2651.910303802808</v>
+      </c>
+      <c r="I41" t="n">
+        <v>6346.186478638949</v>
+      </c>
+      <c r="J41" t="n">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="n">
+        <v>41</v>
+      </c>
+      <c r="B42" t="n">
+        <v>30</v>
+      </c>
+      <c r="C42" t="n">
+        <v>100</v>
+      </c>
+      <c r="D42" t="n">
+        <v>1.14</v>
+      </c>
+      <c r="E42" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t>(-2, -3, -10)</t>
+        </is>
+      </c>
+      <c r="G42" t="n">
+        <v>6484.813541211598</v>
+      </c>
+      <c r="H42" t="n">
+        <v>2650.149083116559</v>
+      </c>
+      <c r="I42" t="n">
+        <v>6370.36495976419</v>
+      </c>
+      <c r="J42" t="n">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="n">
+        <v>42</v>
+      </c>
+      <c r="B43" t="n">
+        <v>30</v>
+      </c>
+      <c r="C43" t="n">
+        <v>250</v>
+      </c>
+      <c r="D43" t="n">
+        <v>1.14</v>
+      </c>
+      <c r="E43" t="n">
+        <v>0.063</v>
+      </c>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>(-2, -3, -10)</t>
+        </is>
+      </c>
+      <c r="G43" t="n">
+        <v>6485.765397728722</v>
+      </c>
+      <c r="H43" t="n">
+        <v>2846.14124767564</v>
+      </c>
+      <c r="I43" t="n">
+        <v>6344.15686905071</v>
+      </c>
+      <c r="J43" t="n">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="n">
+        <v>43</v>
+      </c>
+      <c r="B44" t="n">
+        <v>35</v>
+      </c>
+      <c r="C44" t="n">
+        <v>1</v>
+      </c>
+      <c r="D44" t="n">
+        <v>1.156</v>
+      </c>
+      <c r="E44" t="n">
+        <v>1</v>
+      </c>
+      <c r="F44" t="inlineStr">
+        <is>
+          <t>(-2, -3, -10)</t>
+        </is>
+      </c>
+      <c r="G44" t="n">
+        <v>6410.484684098881</v>
+      </c>
+      <c r="H44" t="n">
+        <v>3239.429882739363</v>
+      </c>
+      <c r="I44" t="n">
+        <v>6461.770673126524</v>
+      </c>
+      <c r="J44" t="n">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="n">
+        <v>44</v>
+      </c>
+      <c r="B45" t="n">
+        <v>35</v>
+      </c>
+      <c r="C45" t="n">
+        <v>5</v>
+      </c>
+      <c r="D45" t="n">
+        <v>1.156</v>
+      </c>
+      <c r="E45" t="n">
+        <v>0.447</v>
+      </c>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>(-2, -3, -10)</t>
+        </is>
+      </c>
+      <c r="G45" t="n">
+        <v>6495.874261947784</v>
+      </c>
+      <c r="H45" t="n">
+        <v>3237.875375303576</v>
+      </c>
+      <c r="I45" t="n">
+        <v>6398.940155616558</v>
+      </c>
+      <c r="J45" t="n">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="n">
+        <v>45</v>
+      </c>
+      <c r="B46" t="n">
+        <v>35</v>
+      </c>
+      <c r="C46" t="n">
+        <v>10</v>
+      </c>
+      <c r="D46" t="n">
+        <v>1.156</v>
+      </c>
+      <c r="E46" t="n">
+        <v>0.316</v>
+      </c>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>(-2, -3, -10)</t>
+        </is>
+      </c>
+      <c r="G46" t="n">
+        <v>6443.174728603133</v>
+      </c>
+      <c r="H46" t="n">
+        <v>2560.03040274042</v>
+      </c>
+      <c r="I46" t="n">
+        <v>6377.351317568551</v>
+      </c>
+      <c r="J46" t="n">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="n">
+        <v>46</v>
+      </c>
+      <c r="B47" t="n">
+        <v>35</v>
+      </c>
+      <c r="C47" t="n">
+        <v>20</v>
+      </c>
+      <c r="D47" t="n">
+        <v>1.156</v>
+      </c>
+      <c r="E47" t="n">
+        <v>0.224</v>
+      </c>
+      <c r="F47" t="inlineStr">
+        <is>
+          <t>(-2, -3, -10)</t>
+        </is>
+      </c>
+      <c r="G47" t="n">
+        <v>6480.817648816126</v>
+      </c>
+      <c r="H47" t="n">
+        <v>2484.359109016109</v>
+      </c>
+      <c r="I47" t="n">
+        <v>6324.747802314831</v>
+      </c>
+      <c r="J47" t="n">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="n">
+        <v>47</v>
+      </c>
+      <c r="B48" t="n">
+        <v>35</v>
+      </c>
+      <c r="C48" t="n">
+        <v>50</v>
+      </c>
+      <c r="D48" t="n">
+        <v>1.156</v>
+      </c>
+      <c r="E48" t="n">
+        <v>0.141</v>
+      </c>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t>(-2, -3, -10)</t>
+        </is>
+      </c>
+      <c r="G48" t="n">
+        <v>6473.408289368143</v>
+      </c>
+      <c r="H48" t="n">
+        <v>3294.725414861646</v>
+      </c>
+      <c r="I48" t="n">
+        <v>6335.231408067987</v>
+      </c>
+      <c r="J48" t="n">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="n">
+        <v>48</v>
+      </c>
+      <c r="B49" t="n">
+        <v>35</v>
+      </c>
+      <c r="C49" t="n">
+        <v>100</v>
+      </c>
+      <c r="D49" t="n">
+        <v>1.156</v>
+      </c>
+      <c r="E49" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F49" t="inlineStr">
+        <is>
+          <t>(-2, -3, -10)</t>
+        </is>
+      </c>
+      <c r="G49" t="n">
+        <v>6468.2382160633</v>
+      </c>
+      <c r="H49" t="n">
+        <v>2855.898655986871</v>
+      </c>
+      <c r="I49" t="n">
+        <v>6380.429115858692</v>
+      </c>
+      <c r="J49" t="n">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="n">
+        <v>49</v>
+      </c>
+      <c r="B50" t="n">
+        <v>35</v>
+      </c>
+      <c r="C50" t="n">
+        <v>250</v>
+      </c>
+      <c r="D50" t="n">
+        <v>1.156</v>
+      </c>
+      <c r="E50" t="n">
+        <v>0.063</v>
+      </c>
+      <c r="F50" t="inlineStr">
+        <is>
+          <t>(-2, -3, -10)</t>
+        </is>
+      </c>
+      <c r="G50" t="n">
+        <v>6444.151649910884</v>
+      </c>
+      <c r="H50" t="n">
+        <v>3098.643561423766</v>
+      </c>
+      <c r="I50" t="n">
+        <v>6293.697471164851</v>
+      </c>
+      <c r="J50" t="n">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="n">
+        <v>50</v>
+      </c>
+      <c r="B51" t="n">
+        <v>40</v>
+      </c>
+      <c r="C51" t="n">
+        <v>1</v>
+      </c>
+      <c r="D51" t="n">
+        <v>1.169</v>
+      </c>
+      <c r="E51" t="n">
+        <v>1</v>
+      </c>
+      <c r="F51" t="inlineStr">
+        <is>
+          <t>(-2, -3, -10)</t>
+        </is>
+      </c>
+      <c r="G51" t="n">
+        <v>6475.869099983413</v>
+      </c>
+      <c r="H51" t="n">
+        <v>2870.088603013452</v>
+      </c>
+      <c r="I51" t="n">
+        <v>6498.4602505251</v>
+      </c>
+      <c r="J51" t="n">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="n">
+        <v>51</v>
+      </c>
+      <c r="B52" t="n">
+        <v>40</v>
+      </c>
+      <c r="C52" t="n">
+        <v>5</v>
+      </c>
+      <c r="D52" t="n">
+        <v>1.169</v>
+      </c>
+      <c r="E52" t="n">
+        <v>0.447</v>
+      </c>
+      <c r="F52" t="inlineStr">
+        <is>
+          <t>(-2, -3, -10)</t>
+        </is>
+      </c>
+      <c r="G52" t="n">
+        <v>6514.285841587563</v>
+      </c>
+      <c r="H52" t="n">
+        <v>2718.175180216841</v>
+      </c>
+      <c r="I52" t="n">
+        <v>6392.876546082497</v>
+      </c>
+      <c r="J52" t="n">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="n">
+        <v>52</v>
+      </c>
+      <c r="B53" t="n">
+        <v>40</v>
+      </c>
+      <c r="C53" t="n">
+        <v>10</v>
+      </c>
+      <c r="D53" t="n">
+        <v>1.169</v>
+      </c>
+      <c r="E53" t="n">
+        <v>0.316</v>
+      </c>
+      <c r="F53" t="inlineStr">
+        <is>
+          <t>(-2, -3, -10)</t>
+        </is>
+      </c>
+      <c r="G53" t="n">
+        <v>6434.506604912761</v>
+      </c>
+      <c r="H53" t="n">
+        <v>3865.107750320235</v>
+      </c>
+      <c r="I53" t="n">
+        <v>6430.894610826233</v>
+      </c>
+      <c r="J53" t="n">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="n">
+        <v>53</v>
+      </c>
+      <c r="B54" t="n">
+        <v>40</v>
+      </c>
+      <c r="C54" t="n">
+        <v>20</v>
+      </c>
+      <c r="D54" t="n">
+        <v>1.169</v>
+      </c>
+      <c r="E54" t="n">
+        <v>0.224</v>
+      </c>
+      <c r="F54" t="inlineStr">
+        <is>
+          <t>(-2, -3, -10)</t>
+        </is>
+      </c>
+      <c r="G54" t="n">
+        <v>6486.67751578781</v>
+      </c>
+      <c r="H54" t="n">
+        <v>2959.006986386817</v>
+      </c>
+      <c r="I54" t="n">
+        <v>6323.155105712735</v>
+      </c>
+      <c r="J54" t="n">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="n">
+        <v>54</v>
+      </c>
+      <c r="B55" t="n">
+        <v>40</v>
+      </c>
+      <c r="C55" t="n">
+        <v>50</v>
+      </c>
+      <c r="D55" t="n">
+        <v>1.169</v>
+      </c>
+      <c r="E55" t="n">
+        <v>0.141</v>
+      </c>
+      <c r="F55" t="inlineStr">
+        <is>
+          <t>(-2, -3, -10)</t>
+        </is>
+      </c>
+      <c r="G55" t="n">
+        <v>6453.081943241586</v>
+      </c>
+      <c r="H55" t="n">
+        <v>2562.798439105787</v>
+      </c>
+      <c r="I55" t="n">
+        <v>6386.219504388487</v>
+      </c>
+      <c r="J55" t="n">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="n">
+        <v>55</v>
+      </c>
+      <c r="B56" t="n">
+        <v>40</v>
+      </c>
+      <c r="C56" t="n">
+        <v>100</v>
+      </c>
+      <c r="D56" t="n">
+        <v>1.169</v>
+      </c>
+      <c r="E56" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F56" t="inlineStr">
+        <is>
+          <t>(-2, -3, -10)</t>
+        </is>
+      </c>
+      <c r="G56" t="n">
+        <v>6484.589570775657</v>
+      </c>
+      <c r="H56" t="n">
+        <v>3202.059674581489</v>
+      </c>
+      <c r="I56" t="n">
+        <v>6333.051262878763</v>
+      </c>
+      <c r="J56" t="n">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="n">
+        <v>56</v>
+      </c>
+      <c r="B57" t="n">
+        <v>40</v>
+      </c>
+      <c r="C57" t="n">
+        <v>250</v>
+      </c>
+      <c r="D57" t="n">
+        <v>1.169</v>
+      </c>
+      <c r="E57" t="n">
+        <v>0.063</v>
+      </c>
+      <c r="F57" t="inlineStr">
+        <is>
+          <t>(-2, -3, -10)</t>
+        </is>
+      </c>
+      <c r="G57" t="n">
+        <v>6436.941777621126</v>
+      </c>
+      <c r="H57" t="n">
+        <v>2572.586093407371</v>
+      </c>
+      <c r="I57" t="n">
+        <v>6358.653392224182</v>
+      </c>
+      <c r="J57" t="n">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="n">
+        <v>57</v>
+      </c>
+      <c r="B58" t="n">
+        <v>50</v>
+      </c>
+      <c r="C58" t="n">
+        <v>1</v>
+      </c>
+      <c r="D58" t="n">
+        <v>1.191</v>
+      </c>
+      <c r="E58" t="n">
+        <v>1</v>
+      </c>
+      <c r="F58" t="inlineStr">
+        <is>
+          <t>(-2, -3, -10)</t>
+        </is>
+      </c>
+      <c r="G58" t="n">
+        <v>6468.855646246679</v>
+      </c>
+      <c r="H58" t="n">
+        <v>3445.324021916562</v>
+      </c>
+      <c r="I58" t="n">
+        <v>6381.097696245396</v>
+      </c>
+      <c r="J58" t="n">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="n">
+        <v>58</v>
+      </c>
+      <c r="B59" t="n">
+        <v>50</v>
+      </c>
+      <c r="C59" t="n">
+        <v>5</v>
+      </c>
+      <c r="D59" t="n">
+        <v>1.191</v>
+      </c>
+      <c r="E59" t="n">
+        <v>0.447</v>
+      </c>
+      <c r="F59" t="inlineStr">
+        <is>
+          <t>(-2, -3, -10)</t>
+        </is>
+      </c>
+      <c r="G59" t="n">
+        <v>6420.666387683262</v>
+      </c>
+      <c r="H59" t="n">
+        <v>2780.176865355665</v>
+      </c>
+      <c r="I59" t="n">
+        <v>6380.242235853793</v>
+      </c>
+      <c r="J59" t="n">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="n">
+        <v>59</v>
+      </c>
+      <c r="B60" t="n">
+        <v>50</v>
+      </c>
+      <c r="C60" t="n">
+        <v>10</v>
+      </c>
+      <c r="D60" t="n">
+        <v>1.191</v>
+      </c>
+      <c r="E60" t="n">
+        <v>0.316</v>
+      </c>
+      <c r="F60" t="inlineStr">
+        <is>
+          <t>(-2, -3, -10)</t>
+        </is>
+      </c>
+      <c r="G60" t="n">
+        <v>6510.870331687431</v>
+      </c>
+      <c r="H60" t="n">
+        <v>2800.731351275695</v>
+      </c>
+      <c r="I60" t="n">
+        <v>6430.731351275695</v>
+      </c>
+      <c r="J60" t="n">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="n">
+        <v>60</v>
+      </c>
+      <c r="B61" t="n">
+        <v>50</v>
+      </c>
+      <c r="C61" t="n">
+        <v>20</v>
+      </c>
+      <c r="D61" t="n">
+        <v>1.191</v>
+      </c>
+      <c r="E61" t="n">
+        <v>0.224</v>
+      </c>
+      <c r="F61" t="inlineStr">
+        <is>
+          <t>(-2, -3, -10)</t>
+        </is>
+      </c>
+      <c r="G61" t="n">
+        <v>6487.216183910024</v>
+      </c>
+      <c r="H61" t="n">
+        <v>3042.822190539747</v>
+      </c>
+      <c r="I61" t="n">
+        <v>6306.609285288754</v>
+      </c>
+      <c r="J61" t="n">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="n">
+        <v>61</v>
+      </c>
+      <c r="B62" t="n">
+        <v>50</v>
+      </c>
+      <c r="C62" t="n">
+        <v>50</v>
+      </c>
+      <c r="D62" t="n">
+        <v>1.191</v>
+      </c>
+      <c r="E62" t="n">
+        <v>0.141</v>
+      </c>
+      <c r="F62" t="inlineStr">
+        <is>
+          <t>(-2, -3, -10)</t>
+        </is>
+      </c>
+      <c r="G62" t="n">
+        <v>6428.512086197366</v>
+      </c>
+      <c r="H62" t="n">
+        <v>3375.705288599639</v>
+      </c>
+      <c r="I62" t="n">
+        <v>6349.420942133346</v>
+      </c>
+      <c r="J62" t="n">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="n">
+        <v>62</v>
+      </c>
+      <c r="B63" t="n">
+        <v>50</v>
+      </c>
+      <c r="C63" t="n">
+        <v>100</v>
+      </c>
+      <c r="D63" t="n">
+        <v>1.191</v>
+      </c>
+      <c r="E63" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F63" t="inlineStr">
+        <is>
+          <t>(-2, -3, -10)</t>
+        </is>
+      </c>
+      <c r="G63" t="n">
+        <v>6445.872380274163</v>
+      </c>
+      <c r="H63" t="n">
+        <v>2841.438002195947</v>
+      </c>
+      <c r="I63" t="n">
+        <v>6359.496758211064</v>
+      </c>
+      <c r="J63" t="n">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="n">
+        <v>63</v>
+      </c>
+      <c r="B64" t="n">
+        <v>50</v>
+      </c>
+      <c r="C64" t="n">
+        <v>250</v>
+      </c>
+      <c r="D64" t="n">
+        <v>1.191</v>
+      </c>
+      <c r="E64" t="n">
+        <v>0.063</v>
+      </c>
+      <c r="F64" t="inlineStr">
+        <is>
+          <t>(-2, -3, -10)</t>
+        </is>
+      </c>
+      <c r="G64" t="n">
+        <v>6458.13651628146</v>
+      </c>
+      <c r="H64" t="n">
+        <v>2974.730396213837</v>
+      </c>
+      <c r="I64" t="n">
+        <v>6308.476595563558</v>
+      </c>
+      <c r="J64" t="n">
         <v>280</v>
       </c>
     </row>

</xml_diff>